<commit_message>
implemented random quirks and updated fear column
</commit_message>
<xml_diff>
--- a/GenNPC.xlsx
+++ b/GenNPC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\pyRepos\NPCgen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB6754-77DF-43DD-AE4E-D280EF104546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF7807A-8AA1-40B2-B1C6-70D49B667EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7DE0866E-C4A5-4E61-BA28-77CED4F27C42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{7DE0866E-C4A5-4E61-BA28-77CED4F27C42}"/>
   </bookViews>
   <sheets>
     <sheet name="Appearance" sheetId="1" r:id="rId1"/>
@@ -486,27 +486,6 @@
     <t>Fears</t>
   </si>
   <si>
-    <t>Heights</t>
-  </si>
-  <si>
-    <t>The dark</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
-    <t>Water/Ocean</t>
-  </si>
-  <si>
-    <t>Snakes</t>
-  </si>
-  <si>
-    <t>Spiders</t>
-  </si>
-  <si>
-    <t>Holes</t>
-  </si>
-  <si>
     <t>Agoraphobia</t>
   </si>
   <si>
@@ -628,6 +607,27 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>Fear of the dark</t>
+  </si>
+  <si>
+    <t>Fear of fire</t>
+  </si>
+  <si>
+    <t>Fear of heights</t>
+  </si>
+  <si>
+    <t>Fear of water/the ocean</t>
+  </si>
+  <si>
+    <t>Fear of snakes</t>
+  </si>
+  <si>
+    <t>Fear of spiders</t>
+  </si>
+  <si>
+    <t>Fear of holes</t>
   </si>
 </sst>
 </file>
@@ -992,7 +992,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1321,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2F5D45-E4BE-4A32-932E-07B791413161}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31:A34"/>
     </sheetView>
   </sheetViews>
@@ -1329,7 +1329,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1517,33 +1517,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>137</v>
@@ -1551,33 +1551,33 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
         <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
         <v>139</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>133</v>
@@ -1594,7 +1594,7 @@
         <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
         <v>140</v>
@@ -1605,13 +1605,13 @@
         <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
         <v>138</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
         <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
         <v>141</v>
@@ -1653,16 +1653,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
         <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
         <v>143</v>
@@ -1676,18 +1676,18 @@
         <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
         <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1724,12 +1724,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD5DF06-89AB-47DB-BC57-07767116191D}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,67 +1752,67 @@
         <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>